<commit_message>
CPU schematics actualizado con el mismo MCU del launchpad y quitado el mux Movidos los pines en el pinout del MCU para hacerlos más compatibles con el launchpad ;)
</commit_message>
<xml_diff>
--- a/IRIS2/01-Design/schematics/IRIS2_pinouts.xlsx
+++ b/IRIS2/01-Design/schematics/IRIS2_pinouts.xlsx
@@ -42,6 +42,15 @@
     <t xml:space="preserve">P1.0/TA0.1/DMAE0/RTCCLK/A0/C0/VREF-/VeREF</t>
   </si>
   <si>
+    <t xml:space="preserve">P1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEBUG_LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug led</t>
+  </si>
+  <si>
     <t xml:space="preserve">P1.1/TA0.2/TA1CLK/COUT/A1/C1/VREF+/VeREF+</t>
   </si>
   <si>
@@ -49,15 +58,6 @@
   </si>
   <si>
     <t xml:space="preserve">P3.0/A12/C12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEBUG_LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Debug led</t>
   </si>
   <si>
     <t xml:space="preserve">P3.1/A13/C13</t>
@@ -724,6 +724,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -745,12 +746,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -760,7 +763,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -770,13 +773,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor rgb="FFFFE699"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE699"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FF3FAF46"/>
+        <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66CC"/>
+        <bgColor rgb="FFFF99CC"/>
       </patternFill>
     </fill>
     <fill>
@@ -794,25 +803,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF66FFFF"/>
-        <bgColor rgb="FF9DC3E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9DC3E6"/>
-        <bgColor rgb="FFBFBFBF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF66CC"/>
-        <bgColor rgb="FFFF99CC"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
-        <bgColor rgb="FF9DC3E6"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -856,9 +853,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -891,19 +890,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -970,13 +961,13 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFE699"/>
-      <rgbColor rgb="FF9DC3E6"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF66FFFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFC7CE"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF66FFFF"/>
+      <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
@@ -984,7 +975,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF3FAF46"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -1006,15 +997,15 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.36"/>
   </cols>
   <sheetData>
@@ -1042,9 +1033,15 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -1052,7 +1049,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1064,7 +1061,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1076,17 +1073,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -1135,7 +1126,7 @@
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -1153,7 +1144,7 @@
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -1279,7 +1270,7 @@
       <c r="C20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -1297,7 +1288,7 @@
       <c r="C21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -1315,7 +1306,7 @@
       <c r="C22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="7" t="s">
         <v>36</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -1333,7 +1324,7 @@
       <c r="C23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="7" t="s">
         <v>39</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -1351,7 +1342,7 @@
       <c r="C24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -1369,7 +1360,7 @@
       <c r="C25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="7" t="s">
         <v>43</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -1423,7 +1414,7 @@
       <c r="C29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -1441,7 +1432,7 @@
       <c r="C30" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -1459,7 +1450,7 @@
       <c r="C31" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E31" s="2" t="s">
@@ -1543,7 +1534,7 @@
       <c r="C36" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="4" t="s">
         <v>73</v>
       </c>
       <c r="E36" s="2" t="s">
@@ -1561,7 +1552,7 @@
       <c r="C37" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="4" t="s">
         <v>76</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -1579,7 +1570,7 @@
       <c r="C38" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="7" t="s">
         <v>80</v>
       </c>
       <c r="E38" s="2" t="s">
@@ -1597,7 +1588,7 @@
       <c r="C39" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="7" t="s">
         <v>84</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -1615,7 +1606,7 @@
       <c r="C40" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E40" s="2" t="s">
@@ -1633,7 +1624,7 @@
       <c r="C41" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -1651,7 +1642,7 @@
       <c r="C42" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E42" s="2" t="s">
@@ -1669,7 +1660,7 @@
       <c r="C43" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E43" s="2" t="s">
@@ -1699,7 +1690,7 @@
       <c r="C45" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="3" t="s">
         <v>96</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -1717,7 +1708,7 @@
       <c r="C46" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="3" t="s">
         <v>99</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -1735,7 +1726,7 @@
       <c r="C47" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -1807,7 +1798,7 @@
       <c r="C52" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="D52" s="8" t="s">
         <v>113</v>
       </c>
       <c r="E52" s="2" t="s">
@@ -1825,7 +1816,7 @@
       <c r="C53" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D53" s="9" t="s">
+      <c r="D53" s="8" t="s">
         <v>117</v>
       </c>
       <c r="E53" s="2" t="s">
@@ -1843,7 +1834,7 @@
       <c r="C54" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="9" t="s">
         <v>121</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -1861,7 +1852,7 @@
       <c r="C55" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D55" s="9" t="s">
         <v>125</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -1879,7 +1870,7 @@
       <c r="C56" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="D56" s="9" t="s">
         <v>129</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -1897,7 +1888,7 @@
       <c r="C57" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="3" t="s">
         <v>132</v>
       </c>
       <c r="E57" s="2" t="s">
@@ -1915,7 +1906,7 @@
       <c r="C58" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="3" t="s">
         <v>136</v>
       </c>
       <c r="E58" s="2" t="s">
@@ -1933,7 +1924,7 @@
       <c r="C59" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="3" t="s">
         <v>139</v>
       </c>
       <c r="E59" s="2" t="s">
@@ -1951,7 +1942,7 @@
       <c r="C60" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="3" t="s">
         <v>142</v>
       </c>
       <c r="E60" s="2" t="s">
@@ -1969,7 +1960,7 @@
       <c r="C61" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E61" s="2" t="s">
@@ -1987,7 +1978,7 @@
       <c r="C62" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E62" s="2" t="s">
@@ -2030,7 +2021,7 @@
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
         <f aca="false">A65+1</f>
         <v>65</v>
@@ -2041,14 +2032,14 @@
       <c r="C66" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D66" s="11" t="s">
+      <c r="D66" s="4" t="s">
         <v>151</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
         <f aca="false">A66+1</f>
         <v>66</v>
@@ -2059,7 +2050,7 @@
       <c r="C67" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D67" s="4" t="s">
         <v>155</v>
       </c>
       <c r="E67" s="2" t="s">
@@ -2149,7 +2140,7 @@
       <c r="C74" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D74" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E74" s="2" t="s">
@@ -2191,7 +2182,7 @@
       <c r="C77" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E77" s="2" t="s">
@@ -2245,7 +2236,7 @@
       <c r="C80" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E80" s="2" t="s">
@@ -2263,7 +2254,7 @@
       <c r="C81" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E81" s="2" t="s">
@@ -2292,7 +2283,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
@@ -2327,40 +2318,40 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="10" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2526,9 +2517,9 @@
       <c r="C7" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
       <c r="I7" s="2" t="n">
         <v>5</v>
       </c>
@@ -2592,13 +2583,13 @@
       <c r="C9" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="10" t="s">
         <v>178</v>
       </c>
       <c r="I9" s="2" t="n">
@@ -2610,9 +2601,9 @@
       <c r="K9" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -2642,9 +2633,9 @@
       <c r="K10" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -2674,9 +2665,9 @@
       <c r="K11" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -2704,14 +2695,14 @@
         <v>205</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
       <c r="E13" s="2" t="n">
         <v>4</v>
       </c>
@@ -2723,48 +2714,48 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="E15" s="14" t="s">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="E15" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="I15" s="14" t="s">
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="I15" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="10" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3086,7 +3077,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -3105,7 +3096,7 @@
       <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.19"/>
@@ -3125,38 +3116,38 @@
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="10" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3266,7 +3257,7 @@
         <f aca="false">A20</f>
         <v>4</v>
       </c>
-      <c r="F6" s="15" t="str">
+      <c r="F6" s="13" t="str">
         <f aca="false">B20</f>
         <v>5V</v>
       </c>
@@ -3431,38 +3422,38 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="10" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3707,9 +3698,9 @@
       <c r="K24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
       <c r="I25" s="2" t="n">
         <v>9</v>
       </c>
@@ -3719,9 +3710,9 @@
       <c r="K25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
       <c r="I26" s="2" t="n">
         <v>10</v>
       </c>
@@ -3777,7 +3768,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>

<commit_message>
Updating the pinout document with the missing parts
</commit_message>
<xml_diff>
--- a/IRIS2/01-Design/schematics/IRIS2_pinouts.xlsx
+++ b/IRIS2/01-Design/schematics/IRIS2_pinouts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="233">
   <si>
     <t xml:space="preserve">Pin</t>
   </si>
@@ -309,6 +309,15 @@
     <t xml:space="preserve">P2.2/TB0.2/UCB0CLK</t>
   </si>
   <si>
+    <t xml:space="preserve">P2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUNRISE_CMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Command from SunRise</t>
+  </si>
+  <si>
     <t xml:space="preserve">P8.1</t>
   </si>
   <si>
@@ -660,55 +669,58 @@
     <t xml:space="preserve">Output</t>
   </si>
   <si>
+    <t xml:space="preserve">Camera 01 IF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART Debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rx from MCU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tx from MCU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power On</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Front Plate Power</t>
+  </si>
+  <si>
     <t xml:space="preserve">Camera 02 IF</t>
   </si>
   <si>
-    <t xml:space="preserve">UART Debug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TXD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rx from MCU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RXD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tx from MCU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camera 01 IF</t>
+    <t xml:space="preserve">JTAG MSP430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDO/TDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vcc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDI/Vpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vcc Ext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST/Vpp</t>
   </si>
   <si>
     <t xml:space="preserve">Camera 03 IF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JTAG MSP430</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TDO/TDI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vcc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TDI/Vpp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vcc Ext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST/Vpp</t>
   </si>
 </sst>
 </file>
@@ -763,7 +775,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -804,6 +816,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF66FFFF"/>
         <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -857,7 +875,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -890,11 +908,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -997,15 +1019,15 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.36"/>
   </cols>
   <sheetData>
@@ -1468,7 +1490,7 @@
       <c r="C32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="8" t="s">
         <v>61</v>
       </c>
       <c r="E32" s="2" t="s">
@@ -1486,7 +1508,7 @@
       <c r="C33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E33" s="2" t="s">
@@ -1504,7 +1526,7 @@
       <c r="C34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="8" t="s">
         <v>69</v>
       </c>
       <c r="E34" s="2" t="s">
@@ -1675,9 +1697,15 @@
       <c r="B44" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
@@ -1685,16 +1713,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,16 +1731,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1721,16 +1749,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1739,7 +1767,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -1751,7 +1779,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -1763,7 +1791,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -1775,16 +1803,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1793,16 +1821,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1811,16 +1839,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>117</v>
+        <v>119</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>120</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1829,16 +1857,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>121</v>
+        <v>123</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1847,16 +1875,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,16 +1893,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>132</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1883,16 +1911,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,16 +1929,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1919,16 +1947,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1937,16 +1965,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1955,10 +1983,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>31</v>
@@ -1973,10 +2001,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>34</v>
@@ -1991,7 +2019,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -2003,7 +2031,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -2015,7 +2043,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -2027,16 +2055,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,16 +2073,16 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2063,7 +2091,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -2075,7 +2103,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -2087,7 +2115,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -2099,7 +2127,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
@@ -2111,7 +2139,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -2123,7 +2151,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -2135,10 +2163,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>31</v>
@@ -2153,7 +2181,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
@@ -2165,7 +2193,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
@@ -2177,10 +2205,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>31</v>
@@ -2195,16 +2223,16 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2213,16 +2241,16 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,10 +2259,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>31</v>
@@ -2249,10 +2277,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>34</v>
@@ -2280,10 +2308,10 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
@@ -2297,62 +2325,62 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="I2" s="10" t="s">
+      <c r="G2" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="M2" s="10" t="s">
+      <c r="K2" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="10" t="s">
-        <v>178</v>
+      <c r="O2" s="11" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2363,7 +2391,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>1</v>
@@ -2372,7 +2400,7 @@
         <v>31</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>1</v>
@@ -2381,16 +2409,16 @@
         <v>31</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="M3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2398,10 +2426,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>2</v>
@@ -2410,25 +2438,25 @@
         <v>31</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="M4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2436,37 +2464,37 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="M5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2477,34 +2505,34 @@
         <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="M6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2515,28 +2543,28 @@
         <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+        <v>182</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
       <c r="I7" s="2" t="n">
         <v>5</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="M7" s="2" t="n">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2547,10 +2575,10 @@
         <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -2558,19 +2586,19 @@
         <v>6</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="M8" s="2" t="n">
         <v>6</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2578,42 +2606,42 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E9" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>178</v>
+      <c r="G9" s="11" t="s">
+        <v>181</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>7</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
+        <v>182</v>
+      </c>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>1</v>
@@ -2622,30 +2650,30 @@
         <v>31</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="I10" s="2" t="n">
         <v>8</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
+        <v>182</v>
+      </c>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>2</v>
@@ -2654,109 +2682,109 @@
         <v>31</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="I11" s="2" t="n">
         <v>9</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
+        <v>182</v>
+      </c>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="I12" s="2" t="n">
         <v>10</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
       <c r="E13" s="2" t="n">
         <v>4</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="E15" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="I15" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="A15" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="E15" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="I15" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="C16" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="I16" s="10" t="s">
+      <c r="G16" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="10" t="s">
-        <v>178</v>
+      <c r="K16" s="11" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2767,23 +2795,23 @@
         <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="G17" s="2"/>
       <c r="I17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2791,26 +2819,26 @@
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="G18" s="2"/>
       <c r="I18" s="2" t="n">
         <v>2</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2818,26 +2846,26 @@
         <v>3</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="G19" s="2"/>
       <c r="I19" s="2" t="n">
         <v>3</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2845,24 +2873,24 @@
         <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C20" s="2"/>
       <c r="E20" s="2" t="n">
         <v>4</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="G20" s="2"/>
       <c r="I20" s="2" t="n">
         <v>4</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2873,7 +2901,7 @@
         <v>34</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>5</v>
@@ -2886,10 +2914,10 @@
         <v>5</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2900,7 +2928,7 @@
         <v>31</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>6</v>
@@ -2913,10 +2941,10 @@
         <v>6</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2927,7 +2955,7 @@
         <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>7</v>
@@ -2940,10 +2968,10 @@
         <v>7</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2954,23 +2982,23 @@
         <v>80</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>8</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="G24" s="2"/>
       <c r="I24" s="2" t="n">
         <v>8</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2978,14 +3006,14 @@
         <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C25" s="2"/>
       <c r="E25" s="2" t="n">
         <v>9</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="G25" s="2"/>
       <c r="I25" s="2" t="n">
@@ -2995,7 +3023,7 @@
         <v>31</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3003,10 +3031,10 @@
         <v>10</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3014,10 +3042,10 @@
         <v>11</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3025,10 +3053,10 @@
         <v>12</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3036,10 +3064,10 @@
         <v>13</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3047,10 +3075,10 @@
         <v>14</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3058,10 +3086,10 @@
         <v>15</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3090,13 +3118,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.19"/>
@@ -3107,48 +3135,48 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="I1" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="I1" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="I2" s="10" t="s">
+      <c r="G2" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="10" t="s">
-        <v>178</v>
+      <c r="K2" s="11" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3159,19 +3187,16 @@
         <v>31</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E3" s="2" t="n">
-        <f aca="false">A17</f>
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="str">
-        <f aca="false">B17</f>
-        <v>GND</v>
-      </c>
-      <c r="G3" s="2" t="str">
-        <f aca="false">C17</f>
-        <v>Out</v>
+      <c r="F3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>1</v>
@@ -3180,7 +3205,7 @@
         <v>31</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3188,28 +3213,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="E4" s="2" t="n">
-        <f aca="false">A18</f>
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="str">
-        <f aca="false">B18</f>
-        <v>GND</v>
-      </c>
-      <c r="G4" s="2" t="str">
-        <f aca="false">C18</f>
-        <v>Out</v>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="K4" s="2"/>
     </row>
@@ -3218,28 +3240,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="E5" s="2" t="n">
-        <f aca="false">A19</f>
         <v>3</v>
       </c>
-      <c r="F5" s="2" t="str">
-        <f aca="false">B19</f>
-        <v>5V</v>
-      </c>
-      <c r="G5" s="2" t="str">
-        <f aca="false">C19</f>
-        <v>Out</v>
+      <c r="F5" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -3251,31 +3270,28 @@
         <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E6" s="2" t="n">
-        <f aca="false">A20</f>
         <v>4</v>
       </c>
-      <c r="F6" s="13" t="str">
-        <f aca="false">B20</f>
-        <v>5V</v>
-      </c>
-      <c r="G6" s="2" t="str">
-        <f aca="false">C20</f>
-        <v>Out</v>
+      <c r="F6" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3286,31 +3302,28 @@
         <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E7" s="2" t="n">
-        <f aca="false">A21</f>
         <v>5</v>
       </c>
-      <c r="F7" s="2" t="str">
-        <f aca="false">B21</f>
-        <v>UART Tx</v>
-      </c>
-      <c r="G7" s="2" t="str">
-        <f aca="false">C21</f>
-        <v>Out</v>
+      <c r="F7" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>5</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3321,25 +3334,22 @@
         <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E8" s="2" t="n">
-        <f aca="false">A22</f>
         <v>6</v>
       </c>
-      <c r="F8" s="2" t="str">
-        <f aca="false">B22</f>
-        <v>UART Rx</v>
-      </c>
-      <c r="G8" s="2" t="str">
-        <f aca="false">C22</f>
-        <v>In</v>
+      <c r="F8" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="I8" s="2" t="n">
         <v>6</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -3348,22 +3358,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E9" s="2" t="n">
-        <f aca="false">A23</f>
         <v>7</v>
       </c>
-      <c r="F9" s="2" t="str">
-        <f aca="false">B23</f>
-        <v>Power On</v>
-      </c>
-      <c r="G9" s="2" t="str">
-        <f aca="false">C23</f>
-        <v>Out</v>
+      <c r="F9" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3371,22 +3378,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E10" s="2" t="n">
-        <f aca="false">A24</f>
         <v>8</v>
       </c>
-      <c r="F10" s="2" t="str">
-        <f aca="false">B24</f>
-        <v>Power Status</v>
-      </c>
-      <c r="G10" s="2" t="str">
-        <f aca="false">C24</f>
-        <v>In</v>
+      <c r="F10" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3394,10 +3398,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3405,56 +3409,56 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="I15" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="I15" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="C16" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="I16" s="10" t="s">
+      <c r="G16" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="10" t="s">
-        <v>178</v>
+      <c r="K16" s="11" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3465,25 +3469,25 @@
         <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="E17" s="2" t="n">
-        <f aca="false">A17</f>
+        <f aca="false">E3</f>
         <v>1</v>
       </c>
       <c r="F17" s="2" t="str">
-        <f aca="false">B17</f>
+        <f aca="false">F3</f>
         <v>GND</v>
       </c>
       <c r="G17" s="2" t="str">
-        <f aca="false">C17</f>
+        <f aca="false">G3</f>
         <v>Out</v>
       </c>
       <c r="I17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="K17" s="2"/>
     </row>
@@ -3495,25 +3499,25 @@
         <v>31</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="E18" s="2" t="n">
-        <f aca="false">A18</f>
+        <f aca="false">E4</f>
         <v>2</v>
       </c>
       <c r="F18" s="2" t="str">
-        <f aca="false">B18</f>
+        <f aca="false">F4</f>
         <v>GND</v>
       </c>
       <c r="G18" s="2" t="str">
-        <f aca="false">C18</f>
+        <f aca="false">G4</f>
         <v>Out</v>
       </c>
       <c r="I18" s="2" t="n">
         <v>2</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="K18" s="2"/>
     </row>
@@ -3522,28 +3526,28 @@
         <v>3</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="E19" s="2" t="n">
-        <f aca="false">A19</f>
+        <f aca="false">E5</f>
         <v>3</v>
       </c>
       <c r="F19" s="2" t="str">
-        <f aca="false">B19</f>
+        <f aca="false">F5</f>
         <v>5V</v>
       </c>
       <c r="G19" s="2" t="str">
-        <f aca="false">C19</f>
+        <f aca="false">G5</f>
         <v>Out</v>
       </c>
       <c r="I19" s="2" t="n">
         <v>3</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="K19" s="2"/>
     </row>
@@ -3552,51 +3556,42 @@
         <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="E20" s="2" t="n">
-        <f aca="false">A20</f>
+        <f aca="false">E6</f>
         <v>4</v>
       </c>
-      <c r="F20" s="2" t="str">
-        <f aca="false">B20</f>
+      <c r="F20" s="14" t="str">
+        <f aca="false">F6</f>
         <v>5V</v>
       </c>
       <c r="G20" s="2" t="str">
-        <f aca="false">C20</f>
+        <f aca="false">G6</f>
         <v>Out</v>
       </c>
       <c r="I20" s="2" t="n">
         <v>4</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="K20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="n">
+      <c r="E21" s="2" t="n">
+        <f aca="false">E7</f>
         <v>5</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <f aca="false">A21</f>
-        <v>5</v>
-      </c>
       <c r="F21" s="2" t="str">
-        <f aca="false">B21</f>
+        <f aca="false">F7</f>
         <v>UART Tx</v>
       </c>
       <c r="G21" s="2" t="str">
-        <f aca="false">C21</f>
+        <f aca="false">G7</f>
         <v>Out</v>
       </c>
       <c r="I21" s="2" t="n">
@@ -3608,55 +3603,37 @@
       <c r="K21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="n">
+      <c r="E22" s="2" t="n">
+        <f aca="false">E8</f>
         <v>6</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E22" s="2" t="n">
-        <f aca="false">A22</f>
-        <v>6</v>
-      </c>
       <c r="F22" s="2" t="str">
-        <f aca="false">B22</f>
+        <f aca="false">F8</f>
         <v>UART Rx</v>
       </c>
       <c r="G22" s="2" t="str">
-        <f aca="false">C22</f>
+        <f aca="false">G8</f>
         <v>In</v>
       </c>
       <c r="I22" s="2" t="n">
         <v>6</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="K22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="n">
+      <c r="E23" s="2" t="n">
+        <f aca="false">E9</f>
         <v>7</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E23" s="2" t="n">
-        <f aca="false">A23</f>
-        <v>7</v>
-      </c>
       <c r="F23" s="2" t="str">
-        <f aca="false">B23</f>
+        <f aca="false">F9</f>
         <v>Power On</v>
       </c>
       <c r="G23" s="2" t="str">
-        <f aca="false">C23</f>
+        <f aca="false">G9</f>
         <v>Out</v>
       </c>
       <c r="I23" s="2" t="n">
@@ -3668,39 +3645,30 @@
       <c r="K23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="n">
+      <c r="E24" s="2" t="n">
+        <f aca="false">E10</f>
         <v>8</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E24" s="2" t="n">
-        <f aca="false">A24</f>
-        <v>8</v>
-      </c>
       <c r="F24" s="2" t="str">
-        <f aca="false">B24</f>
+        <f aca="false">F10</f>
         <v>Power Status</v>
       </c>
       <c r="G24" s="2" t="str">
-        <f aca="false">C24</f>
+        <f aca="false">G10</f>
         <v>In</v>
       </c>
       <c r="I24" s="2" t="n">
         <v>8</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="K24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
       <c r="I25" s="2" t="n">
         <v>9</v>
       </c>
@@ -3710,14 +3678,14 @@
       <c r="K25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
       <c r="I26" s="2" t="n">
         <v>10</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="K26" s="2"/>
     </row>
@@ -3735,36 +3703,163 @@
         <v>12</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="K28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
       <c r="I29" s="2" t="n">
         <v>13</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="K29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>181</v>
+      </c>
       <c r="I30" s="2" t="n">
         <v>14</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="K30" s="2"/>
     </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="2" t="n">
+        <f aca="false">E3</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="str">
+        <f aca="false">F3</f>
+        <v>GND</v>
+      </c>
+      <c r="G31" s="2" t="str">
+        <f aca="false">G3</f>
+        <v>Out</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="2" t="n">
+        <f aca="false">E4</f>
+        <v>2</v>
+      </c>
+      <c r="F32" s="2" t="str">
+        <f aca="false">F4</f>
+        <v>GND</v>
+      </c>
+      <c r="G32" s="2" t="str">
+        <f aca="false">G4</f>
+        <v>Out</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="2" t="n">
+        <f aca="false">E5</f>
+        <v>3</v>
+      </c>
+      <c r="F33" s="2" t="str">
+        <f aca="false">F5</f>
+        <v>5V</v>
+      </c>
+      <c r="G33" s="2" t="str">
+        <f aca="false">G5</f>
+        <v>Out</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="2" t="n">
+        <f aca="false">E6</f>
+        <v>4</v>
+      </c>
+      <c r="F34" s="2" t="str">
+        <f aca="false">F6</f>
+        <v>5V</v>
+      </c>
+      <c r="G34" s="2" t="str">
+        <f aca="false">G6</f>
+        <v>Out</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="2" t="n">
+        <f aca="false">E7</f>
+        <v>5</v>
+      </c>
+      <c r="F35" s="2" t="str">
+        <f aca="false">F7</f>
+        <v>UART Tx</v>
+      </c>
+      <c r="G35" s="2" t="str">
+        <f aca="false">G7</f>
+        <v>Out</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="2" t="n">
+        <f aca="false">E8</f>
+        <v>6</v>
+      </c>
+      <c r="F36" s="2" t="str">
+        <f aca="false">F8</f>
+        <v>UART Rx</v>
+      </c>
+      <c r="G36" s="2" t="str">
+        <f aca="false">G8</f>
+        <v>In</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="2" t="n">
+        <f aca="false">E9</f>
+        <v>7</v>
+      </c>
+      <c r="F37" s="2" t="str">
+        <f aca="false">F9</f>
+        <v>Power On</v>
+      </c>
+      <c r="G37" s="2" t="str">
+        <f aca="false">G9</f>
+        <v>Out</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="2" t="n">
+        <f aca="false">E10</f>
+        <v>8</v>
+      </c>
+      <c r="F38" s="2" t="str">
+        <f aca="false">F10</f>
+        <v>Power Status</v>
+      </c>
+      <c r="G38" s="2" t="str">
+        <f aca="false">G10</f>
+        <v>In</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="I15:K15"/>
+    <mergeCell ref="E29:G29"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added Vin to the debug connector to be able to power up IRIS withtout using the internal batteries Updated pinout excel and added images of the pinouts, corrected the pinout of the Sunrise pins Updated the schematics to support the added Vin pins to the debug connector
</commit_message>
<xml_diff>
--- a/IRIS2/01-Design/schematics/IRIS2_pinouts.xlsx
+++ b/IRIS2/01-Design/schematics/IRIS2_pinouts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bultz\workspace_daedalus\IRIS2\IRIS2\01-Design\IRIS2_PCB_CPU\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bultz\workspace_daedalus\IRIS2\IRIS2\01-Design\schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203DDF37-83D0-493F-A44C-8AFB195AE4C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA636343-925A-495D-A672-7D1740184421}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MCU" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="234">
   <si>
     <t>Pin</t>
   </si>
@@ -735,6 +735,9 @@
   </si>
   <si>
     <t>External I2C SDA for external sensors</t>
+  </si>
+  <si>
+    <t>Vin</t>
   </si>
 </sst>
 </file>
@@ -857,12 +860,6 @@
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -877,6 +874,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Bad" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -961,6 +964,160 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>102577</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>12354</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>417634</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>10258</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B94FC20-C632-429D-BFD7-B714D844F8C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3326423" y="6137662"/>
+          <a:ext cx="3033346" cy="1932211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600810</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14652</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>754305</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>72224</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3042000F-143A-4518-9B8B-2031D5152C97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8792310" y="2593729"/>
+          <a:ext cx="2593360" cy="2636649"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>80596</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>92137</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>14654</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>36327</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D35C136-843A-490D-985B-243ECDA146AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="373673" y="5572675"/>
+          <a:ext cx="2579077" cy="3168037"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1262,7 +1419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
@@ -1277,1276 +1434,1276 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <f t="shared" ref="A3:A34" si="0">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+      <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+      <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+      <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+      <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
+      <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+      <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+      <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+      <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+      <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+      <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
+      <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+      <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
+      <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
+      <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
+      <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
+      <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="4">
+      <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="4">
+      <c r="A34" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
+      <c r="A35" s="2">
         <f t="shared" ref="A35:A66" si="1">A34+1</f>
         <v>34</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="4">
+      <c r="A36" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="4">
+      <c r="A37" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
+      <c r="A38" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
+      <c r="A39" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D39" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="4">
+      <c r="A40" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="4">
+      <c r="A41" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="4">
+      <c r="A42" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="4">
+      <c r="A43" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="4">
+      <c r="A44" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="4">
+      <c r="A45" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="4">
+      <c r="A46" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="4">
+      <c r="A47" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="4">
+      <c r="A48" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="4">
+      <c r="A49" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="4">
+      <c r="A50" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="E50" s="4"/>
+      <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
+      <c r="A51" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="4">
+      <c r="A52" s="2">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D52" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="2" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="4">
+      <c r="A53" s="2">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="D53" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="4">
+      <c r="A54" s="2">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C54" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="4">
+      <c r="A55" s="2">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="C55" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="D55" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="4">
+      <c r="A56" s="2">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C56" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="D56" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="4">
+      <c r="A57" s="2">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E57" s="2" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="4">
+      <c r="A58" s="2">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E58" s="2" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="4">
+      <c r="A59" s="2">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="C59" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E59" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="4">
+      <c r="A60" s="2">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E60" s="2" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="4">
+      <c r="A61" s="2">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="4">
+      <c r="A62" s="2">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="D62" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E62" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="4">
+      <c r="A63" s="2">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="4">
+      <c r="A64" s="2">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="4">
+      <c r="A65" s="2">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C65" s="15"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="4">
+      <c r="A66" s="2">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C66" s="15" t="s">
+      <c r="C66" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E66" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="4">
+      <c r="A67" s="2">
         <f t="shared" ref="A67:A81" si="2">A66+1</f>
         <v>66</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C67" s="15" t="s">
+      <c r="C67" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D67" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E67" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="4">
+      <c r="A68" s="2">
         <f t="shared" si="2"/>
         <v>67</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="4">
+      <c r="A69" s="2">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="4">
+      <c r="A70" s="2">
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="4">
+      <c r="A71" s="2">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="4">
+      <c r="A72" s="2">
         <f t="shared" si="2"/>
         <v>71</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="4">
+      <c r="A73" s="2">
         <f t="shared" si="2"/>
         <v>72</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="4">
+      <c r="A74" s="2">
         <f t="shared" si="2"/>
         <v>73</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D74" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E74" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="4">
+      <c r="A75" s="2">
         <f t="shared" si="2"/>
         <v>74</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="4">
+      <c r="A76" s="2">
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="4">
+      <c r="A77" s="2">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C77" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E77" s="4" t="s">
+      <c r="E77" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="4">
+      <c r="A78" s="2">
         <f t="shared" si="2"/>
         <v>77</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C78" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E78" s="4" t="s">
+      <c r="E78" s="2" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="4">
+      <c r="A79" s="2">
         <f t="shared" si="2"/>
         <v>78</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="C79" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="D79" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E79" s="4" t="s">
+      <c r="E79" s="2" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="4">
+      <c r="A80" s="2">
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="C80" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D80" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E80" s="4" t="s">
+      <c r="E80" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="4">
+      <c r="A81" s="2">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D81" s="8" t="s">
+      <c r="D81" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E81" s="4" t="s">
+      <c r="E81" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2564,8 +2721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2581,791 +2738,796 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="I1" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="M1" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="11" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="2">
         <v>1</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="2" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="2">
         <v>2</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="2">
         <v>2</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="2" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="2">
         <v>3</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="2">
         <v>3</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="2" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>4</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="2">
         <v>4</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="2">
         <v>4</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="2" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="I7" s="4">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="I7" s="2">
         <v>5</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="2">
         <v>5</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="2" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="I8" s="4">
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="I8" s="2">
         <v>6</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="2">
         <v>6</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="2" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="2">
         <v>7</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="2">
         <v>1</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="2">
         <v>8</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="2">
         <v>2</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="2">
         <v>9</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="2">
         <v>3</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="2">
         <v>10</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K12" s="4"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
+      <c r="K12" s="2"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="E13" s="4">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="E13" s="2">
         <v>4</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="2" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="E15" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="I15" s="1" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="I15" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="11" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="A17" s="2">
         <v>1</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="2">
         <v>1</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="I17" s="4">
+      <c r="G17" s="2"/>
+      <c r="I17" s="2">
         <v>1</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="2" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="2">
         <v>2</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="2">
         <v>2</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="I18" s="4">
+      <c r="G18" s="2"/>
+      <c r="I18" s="2">
         <v>2</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="2" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="A19" s="2">
         <v>3</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="2">
         <v>3</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="I19" s="4">
+      <c r="F19" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="I19" s="2">
         <v>3</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="2" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="A20" s="2">
         <v>4</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="E20" s="2">
+        <v>4</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="E20" s="4">
+      <c r="G20" s="2"/>
+      <c r="I20" s="2">
         <v>4</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="J20" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E21" s="2">
+        <v>5</v>
+      </c>
+      <c r="F21" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="I20" s="4">
-        <v>4</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="K20" s="4" t="s">
+      <c r="G21" s="2"/>
+      <c r="I21" s="2">
+        <v>5</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>5</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="4" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E21" s="4">
-        <v>5</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="I21" s="4">
-        <v>5</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="K21" s="4" t="s">
+      <c r="E22" s="2">
+        <v>6</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="I22" s="2">
+        <v>6</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K22" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
-        <v>6</v>
-      </c>
-      <c r="B22" s="4" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E23" s="2">
+        <v>7</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="I23" s="2">
+        <v>7</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E24" s="2">
+        <v>8</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="I24" s="2">
+        <v>8</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>9</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="E25" s="2">
+        <v>9</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="I25" s="2">
+        <v>9</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="K25" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E22" s="4">
-        <v>6</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="I22" s="4">
-        <v>6</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
-        <v>7</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E23" s="4">
-        <v>7</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G23" s="4"/>
-      <c r="I23" s="4">
-        <v>7</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
-        <v>8</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E24" s="4">
-        <v>8</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="G24" s="4"/>
-      <c r="I24" s="4">
-        <v>8</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
-        <v>9</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="E25" s="4">
-        <v>9</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="G25" s="4"/>
-      <c r="I25" s="4">
-        <v>9</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I26" s="4">
+      <c r="I26" s="2">
         <v>10</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K26" s="2" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I27" s="4">
+      <c r="I27" s="2">
         <v>11</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="2" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I28" s="4">
+      <c r="I28" s="2">
         <v>12</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="J28" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K28" s="2" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I29" s="4">
+      <c r="I29" s="2">
         <v>13</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J29" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="2" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I30" s="4">
+      <c r="I30" s="2">
         <v>14</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J30" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="2" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I31" s="4">
+      <c r="I31" s="2">
         <v>15</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="J31" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="K31" s="2" t="s">
         <v>207</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="E8:G8"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="E8:G8"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3387,160 +3549,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="1" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="I1" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="11" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="2">
         <v>2</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K4" s="4"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="2">
         <v>3</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>4</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="2">
         <v>4</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="2" t="s">
         <v>180</v>
       </c>
       <c r="L6" t="s">
@@ -3548,31 +3710,31 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>5</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="2">
         <v>5</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L7" t="s">
@@ -3580,526 +3742,526 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
         <v>6</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="2">
         <v>6</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K8" s="4"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="2">
         <v>7</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="2">
         <v>8</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="E15" s="2" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="E15" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="I15" s="1" t="s">
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="I15" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="11" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="A17" s="2">
         <v>1</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="2">
         <f t="shared" ref="E17:G24" si="0">E3</f>
         <v>1</v>
       </c>
-      <c r="F17" s="4" t="str">
+      <c r="F17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GND</v>
       </c>
-      <c r="G17" s="4" t="str">
+      <c r="G17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="2">
         <v>1</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="K17" s="4"/>
+      <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="2">
         <v>2</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F18" s="4" t="str">
+      <c r="F18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GND</v>
       </c>
-      <c r="G18" s="4" t="str">
+      <c r="G18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="2">
         <v>2</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="K18" s="4"/>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="A19" s="2">
         <v>3</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F19" s="4" t="str">
+      <c r="F19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>5V</v>
       </c>
-      <c r="G19" s="4" t="str">
+      <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="2">
         <v>3</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="K19" s="4"/>
+      <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="A20" s="2">
         <v>4</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F20" s="15" t="str">
+      <c r="F20" s="13" t="str">
         <f t="shared" si="0"/>
         <v>5V</v>
       </c>
-      <c r="G20" s="4" t="str">
+      <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="2">
         <v>4</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="K20" s="4"/>
+      <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E21" s="4">
+      <c r="E21" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F21" s="4" t="str">
+      <c r="F21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UART Tx</v>
       </c>
-      <c r="G21" s="4" t="str">
+      <c r="G21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="2">
         <v>5</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K21" s="4"/>
+      <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E22" s="4">
+      <c r="E22" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F22" s="4" t="str">
+      <c r="F22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UART Rx</v>
       </c>
-      <c r="G22" s="4" t="str">
+      <c r="G22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>In</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="2">
         <v>6</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K22" s="4"/>
+      <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E23" s="4">
+      <c r="E23" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F23" s="4" t="str">
+      <c r="F23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Power On</v>
       </c>
-      <c r="G23" s="4" t="str">
+      <c r="G23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="2">
         <v>7</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K23" s="4"/>
+      <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E24" s="4">
+      <c r="E24" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F24" s="4" t="str">
+      <c r="F24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Power Status</v>
       </c>
-      <c r="G24" s="4" t="str">
+      <c r="G24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>In</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="2">
         <v>8</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="K24" s="4"/>
+      <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="I25" s="4">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="I25" s="2">
         <v>9</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K25" s="4"/>
+      <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="I26" s="4">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="I26" s="2">
         <v>10</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K26" s="4"/>
+      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I27" s="4">
+      <c r="I27" s="2">
         <v>11</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K27" s="4"/>
+      <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I28" s="4">
+      <c r="I28" s="2">
         <v>12</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="J28" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K28" s="4"/>
+      <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="I29" s="4">
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="I29" s="2">
         <v>13</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J29" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K29" s="4"/>
+      <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="2">
         <v>14</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J30" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K30" s="4"/>
+      <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E31" s="4">
+      <c r="E31" s="2">
         <f t="shared" ref="E31:G38" si="1">E3</f>
         <v>1</v>
       </c>
-      <c r="F31" s="4" t="str">
+      <c r="F31" s="2" t="str">
         <f t="shared" si="1"/>
         <v>GND</v>
       </c>
-      <c r="G31" s="4" t="str">
+      <c r="G31" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Out</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E32" s="4">
+      <c r="E32" s="2">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F32" s="4" t="str">
+      <c r="F32" s="2" t="str">
         <f t="shared" si="1"/>
         <v>GND</v>
       </c>
-      <c r="G32" s="4" t="str">
+      <c r="G32" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Out</v>
       </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E33" s="4">
+      <c r="E33" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F33" s="4" t="str">
+      <c r="F33" s="2" t="str">
         <f t="shared" si="1"/>
         <v>5V</v>
       </c>
-      <c r="G33" s="4" t="str">
+      <c r="G33" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Out</v>
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E34" s="4">
+      <c r="E34" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F34" s="4" t="str">
+      <c r="F34" s="2" t="str">
         <f t="shared" si="1"/>
         <v>5V</v>
       </c>
-      <c r="G34" s="4" t="str">
+      <c r="G34" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Out</v>
       </c>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E35" s="4">
+      <c r="E35" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F35" s="4" t="str">
+      <c r="F35" s="2" t="str">
         <f t="shared" si="1"/>
         <v>UART Tx</v>
       </c>
-      <c r="G35" s="4" t="str">
+      <c r="G35" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Out</v>
       </c>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E36" s="4">
+      <c r="E36" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F36" s="4" t="str">
+      <c r="F36" s="2" t="str">
         <f t="shared" si="1"/>
         <v>UART Rx</v>
       </c>
-      <c r="G36" s="4" t="str">
+      <c r="G36" s="2" t="str">
         <f t="shared" si="1"/>
         <v>In</v>
       </c>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E37" s="4">
+      <c r="E37" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="F37" s="4" t="str">
+      <c r="F37" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Power On</v>
       </c>
-      <c r="G37" s="4" t="str">
+      <c r="G37" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Out</v>
       </c>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E38" s="4">
+      <c r="E38" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F38" s="4" t="str">
+      <c r="F38" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Power Status</v>
       </c>
-      <c r="G38" s="4" t="str">
+      <c r="G38" s="2" t="str">
         <f t="shared" si="1"/>
         <v>In</v>
       </c>

</xml_diff>

<commit_message>
Updated datasheets of the components to be used
</commit_message>
<xml_diff>
--- a/IRIS2/01-Design/schematics/IRIS2_pinouts.xlsx
+++ b/IRIS2/01-Design/schematics/IRIS2_pinouts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bultz\workspace_daedalus\IRIS2\IRIS2\01-Design\IRIS2_PCB_CPU\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bultz\workspace_daedalus\IRIS2\IRIS2\01-Design\schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2AD52A-FEFC-4A42-92A2-CFF57F4006B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F198CA6-9608-4889-8909-CABC742EE995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MCU" sheetId="1" r:id="rId1"/>
@@ -698,9 +698,6 @@
     <t>UART Debug</t>
   </si>
   <si>
-    <t>5V</t>
-  </si>
-  <si>
     <t>TXD</t>
   </si>
   <si>
@@ -786,6 +783,9 @@
   </si>
   <si>
     <t>Power from Camera 04 Status (Input)</t>
+  </si>
+  <si>
+    <t>3.9V</t>
   </si>
 </sst>
 </file>
@@ -922,10 +922,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1446,7 +1446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
     </sheetView>
@@ -2470,10 +2470,10 @@
         <v>151</v>
       </c>
       <c r="D63" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -2485,13 +2485,13 @@
         <v>152</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -2503,13 +2503,13 @@
         <v>153</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -2557,13 +2557,13 @@
         <v>160</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -2575,13 +2575,13 @@
         <v>161</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -2778,8 +2778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2795,26 +2795,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="E1" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="I1" s="14" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="I1" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="M1" s="14" t="s">
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="M1" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
@@ -3048,11 +3048,11 @@
       <c r="C8" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="I8" s="2">
         <v>6</v>
       </c>
@@ -3225,21 +3225,21 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="E15" s="13" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="E15" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="I15" s="13" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="I15" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
@@ -3604,8 +3604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3618,21 +3618,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="E1" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="I1" s="13" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="I1" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
@@ -3733,7 +3733,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>220</v>
+        <v>249</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>183</v>
@@ -3760,7 +3760,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>220</v>
+        <v>249</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>183</v>
@@ -3769,13 +3769,13 @@
         <v>4</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>187</v>
       </c>
       <c r="L6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -3801,13 +3801,13 @@
         <v>5</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -3851,7 +3851,7 @@
         <v>7</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>183</v>
@@ -3871,7 +3871,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>187</v>
@@ -3900,21 +3900,21 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="E15" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="E15" s="14" t="s">
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="I15" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="I15" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
@@ -3971,7 +3971,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K17" s="2"/>
     </row>
@@ -4001,7 +4001,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K18" s="2"/>
     </row>
@@ -4021,7 +4021,7 @@
       </c>
       <c r="F19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>5V</v>
+        <v>3.9V</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4031,7 +4031,7 @@
         <v>3</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K19" s="2"/>
     </row>
@@ -4051,7 +4051,7 @@
       </c>
       <c r="F20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>5V</v>
+        <v>3.9V</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4061,7 +4061,7 @@
         <v>4</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K20" s="2"/>
     </row>
@@ -4145,7 +4145,7 @@
         <v>8</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K24" s="2"/>
     </row>
@@ -4192,11 +4192,11 @@
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E29" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="E29" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="I29" s="2">
         <v>13</v>
       </c>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="F33" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>5V</v>
+        <v>3.9V</v>
       </c>
       <c r="G33" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4272,7 +4272,7 @@
       </c>
       <c r="F34" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>5V</v>
+        <v>3.9V</v>
       </c>
       <c r="G34" s="2" t="str">
         <f t="shared" si="1"/>

</xml_diff>